<commit_message>
add some checks for 4th lab
</commit_message>
<xml_diff>
--- a/OERPS/lab4_5/var1.xlsx
+++ b/OERPS/lab4_5/var1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задание" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="189">
   <si>
     <t xml:space="preserve">Предприятие выпускает и реализует котлеты киевские, цыплята фаршированные,  пельмени.</t>
   </si>
@@ -531,542 +531,19 @@
     <t xml:space="preserve">Предприятие</t>
   </si>
   <si>
-    <t xml:space="preserve">Вид оборудования</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Фарш говяжий</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Фарш дом</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Фарш куриный</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Тесто</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Пельмени из говядины</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Пельмени домашние</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Котлета по киевски</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Блины</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Трудоемкость изготовления </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Цыпленок фаршированный</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">нормо-ч./ед</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="12"/>
-        <rFont val="TimesET"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
+    <t xml:space="preserve">Общий объём выпуска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Станкоёмкость изготовления, маш/ч</t>
+  </si>
+  <si>
+    <t xml:space="preserve">процентное соотношение к общему объёму выпуска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">станкоёмкость изготовления условного изделия, маш/ч</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Котлета по киевски</t>
   </si>
   <si>
     <t xml:space="preserve">Годовой календарный фонд, ч</t>
@@ -1150,10 +627,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1228,22 +706,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="12"/>
-      <name val="TimesET"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1253,7 +715,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1276,10 +738,66 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
-      <top style="hair"/>
+      <top style="thin"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -1308,7 +826,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1409,35 +927,63 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1449,8 +995,16 @@
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1476,9 +1030,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4235400</xdr:colOff>
+      <xdr:colOff>4235040</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1492,7 +1046,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1203120" y="2828880"/>
-          <a:ext cx="4149720" cy="6398280"/>
+          <a:ext cx="4149360" cy="6397920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1596,8 +1150,8 @@
   </sheetPr>
   <dimension ref="A3:K66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J68" activeCellId="0" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2985,7 +2539,9 @@
       <c r="H61" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="I61" s="10"/>
+      <c r="I61" s="10" t="n">
+        <v>3</v>
+      </c>
       <c r="J61" s="10" t="s">
         <v>93</v>
       </c>
@@ -3014,7 +2570,9 @@
       <c r="H62" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="I62" s="10"/>
+      <c r="I62" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="J62" s="10" t="s">
         <v>93</v>
       </c>
@@ -4947,17 +4505,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4988,636 +4547,863 @@
       <c r="E4" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="29" t="s">
         <v>156</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
         <v>157</v>
       </c>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="32" t="s">
         <v>158</v>
       </c>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="30" t="s">
         <v>159</v>
       </c>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="32" t="s">
         <v>160</v>
       </c>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="30" t="s">
         <v>161</v>
       </c>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="32" t="s">
         <v>162</v>
       </c>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="32" t="s">
         <v>163</v>
       </c>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="32" t="s">
         <v>164</v>
       </c>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="32" t="s">
         <v>165</v>
       </c>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="32" t="s">
         <v>166</v>
       </c>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="33" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B19" s="0" t="n">
+        <f aca="false">lab4!G12+lab4!G13+lab4!G14</f>
+        <v>973</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="27.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="B21" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I6</f>
+        <v>5</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I24</f>
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I15</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="B22" s="0" t="n">
+        <f aca="false">lab4!G14/B19</f>
+        <v>0.197327852004111</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">lab4!G12/B19</f>
+        <v>0.723535457348407</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">lab4!G13/B19</f>
+        <v>0.079136690647482</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">SUM(B22:D22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="B23" s="38" t="n">
+        <f aca="false">B22*B21+C22*C21+D22*D21</f>
+        <v>4.27646454265159</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">lab4!G12+lab4!G13+lab4!G14</f>
+        <v>973</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I7</f>
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I25</f>
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I16</f>
+        <v>2</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">lab4!G14/B19</f>
+        <v>0.197327852004111</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">lab4!G12/B19</f>
+        <v>0.723535457348407</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">lab4!G13/B19</f>
+        <v>0.079136690647482</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">SUM(B30:D30)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="38" t="n">
+        <f aca="false">B30*B29+C30*C29+D30*D29</f>
+        <v>1.6382322713258</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">lab4!G11</f>
+        <v>279.8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I32</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">lab4!G11/lab4!G11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="38" t="n">
+        <f aca="false">B36*B37</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">lab4!G8+lab4!G9+lab4!G7</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="30" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I39</f>
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I44</f>
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I49</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">lab4!G9/B41</f>
+        <v>0.342857142857143</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">lab4!G8/B41</f>
+        <v>0.104761904761905</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">lab4!G7/B41</f>
+        <v>0.552380952380952</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">SUM(B44:D44)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="38" t="n">
+        <f aca="false">B44*B43+C44*C43+D44*D43</f>
+        <v>0.776190476190476</v>
+      </c>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <f aca="false">=lab4!G8+lab4!G9+lab4!G7</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I40</f>
+        <v>3</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I45</f>
+        <v>3</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I51</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <f aca="false">lab4!G9/B41</f>
+        <v>0.342857142857143</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <f aca="false">lab4!G8/B41</f>
+        <v>0.104761904761905</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <f aca="false">lab4!G7/B41</f>
+        <v>0.552380952380952</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">SUM(B52:D52)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="38" t="n">
+        <f aca="false">B52*B51+C52*C51+D52*D51</f>
+        <v>3</v>
+      </c>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <f aca="false">lab4!G15</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I56</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <f aca="false">lab4!G15/lab4!G15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="38" t="n">
+        <f aca="false">B59*B58</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <f aca="false">=lab4!G22+lab4!G23+lab4!G21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I54</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I59</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <f aca="false">ОсновныеДанные!I65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="0" t="e">
+        <f aca="false">lab4!G23/B55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C66" s="0" t="e">
+        <f aca="false">lab4!G22/B55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D66" s="0" t="e">
+        <f aca="false">lab4!G21/B55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E66" s="0" t="e">
+        <f aca="false">SUM(B66:D66)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="38" t="e">
+        <f aca="false">B66*B65+C66*C65+D66*D65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="G20" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <f aca="false">lab4!G14*ОсновныеДанные!H6 / 100</f>
-        <v>9.6</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <f aca="false">lab4!G13*ОсновныеДанные!H15 / 100</f>
-        <v>3.85</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">lab4!G12*ОсновныеДанные!H24 / 100</f>
-        <v>28.16</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <f aca="false">lab4!G14*ОсновныеДанные!H7 / 100</f>
-        <v>3.84</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <f aca="false">lab4!G13*ОсновныеДанные!H16 / 100</f>
-        <v>1.54</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <f aca="false">lab4!G12*ОсновныеДанные!H25 / 100</f>
-        <v>10.56</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <f aca="false">lab4!G11*ОсновныеДанные!H32 / 10</f>
-        <v>55.96</v>
-      </c>
-      <c r="F23" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="32" t="n">
-        <f aca="false">lab4!G9*ОсновныеДанные!H39 / 10</f>
-        <v>18</v>
-      </c>
-      <c r="G24" s="31" t="n">
-        <f aca="false">lab4!G8*ОсновныеДанные!H44 / 10</f>
-        <v>5.5</v>
-      </c>
-      <c r="H24" s="31" t="n">
-        <f aca="false">lab4!G7*ОсновныеДанные!H49 / 10</f>
-        <v>58</v>
-      </c>
-      <c r="I24" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="32" t="n">
-        <f aca="false">lab4!G9*ОсновныеДанные!H40 / 10</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="31" t="n">
-        <f aca="false">lab4!G8*ОсновныеДанные!H45 / 10</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="31" t="n">
-        <f aca="false">lab4!G7*ОсновныеДанные!H51 / 10</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="31" t="n">
-        <f aca="false">lab4!G15*ОсновныеДанные!H56/ 10</f>
-        <v>2.6</v>
-      </c>
-      <c r="J26" s="31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="31" t="n">
-        <f aca="false">lab4!G10*ОсновныеДанные!H61 / 10 + lab4!G10*ОсновныеДанные!H62</f>
-        <v>286</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B31" s="0" t="n">
+      <c r="B82" s="0" t="n">
         <f aca="false">365 * 24</f>
         <v>8760</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="B88" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B89" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <f aca="false">(B86* (365  - B85) - B88*B89) * B83</f>
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <f aca="false">B91*B87/100</f>
+        <v>118.9</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <f aca="false">B91-B92</f>
+        <v>2259.1</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" s="21" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="0" t="n">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="86.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C106" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="D106" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <f aca="false">B97</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B38" s="0" t="n">
+      <c r="C107" s="0" t="n">
+        <f aca="false">$B$93</f>
+        <v>2259.1</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <f aca="false">C107*B107</f>
+        <v>11295.5</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <f aca="false">B98</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <f aca="false">(B35* (365  - B34) - B37*B38) * B32</f>
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <f aca="false">B40*B36/100</f>
-        <v>118.9</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <f aca="false">B40-B41</f>
+      <c r="C108" s="0" t="n">
+        <f aca="false">$B$93</f>
         <v>2259.1</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="B46" s="21" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="34" t="s">
+      <c r="D108" s="0" t="n">
+        <f aca="false">C108*B108</f>
+        <v>4518.2</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B109" s="0" t="n">
+        <f aca="false">B99</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="34" t="s">
+      <c r="C109" s="0" t="n">
+        <f aca="false">$B$93</f>
+        <v>2259.1</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <f aca="false">C109*B109</f>
+        <v>9036.4</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B110" s="0" t="n">
+        <f aca="false">B100</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="34" t="s">
+      <c r="C110" s="0" t="n">
+        <f aca="false">$B$93</f>
+        <v>2259.1</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <f aca="false">C110*B110</f>
+        <v>13554.6</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B111" s="0" t="n">
+        <f aca="false">B101</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="34" t="s">
+      <c r="C111" s="0" t="n">
+        <f aca="false">$B$93</f>
+        <v>2259.1</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <f aca="false">C111*B111</f>
+        <v>13554.6</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B112" s="0" t="n">
+        <f aca="false">B102</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="34" t="s">
+      <c r="C112" s="0" t="n">
+        <f aca="false">$B$93</f>
+        <v>2259.1</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <f aca="false">C112*B112</f>
+        <v>9036.4</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B113" s="0" t="n">
+        <f aca="false">B103</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="B55" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <f aca="false">B46</f>
-        <v>5</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <f aca="false">$B$42</f>
+      <c r="C113" s="0" t="n">
+        <f aca="false">$B$93</f>
         <v>2259.1</v>
       </c>
-      <c r="D56" s="0" t="n">
-        <f aca="false">C56*B56</f>
-        <v>11295.5</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <f aca="false">B47</f>
-        <v>2</v>
-      </c>
-      <c r="C57" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <f aca="false">C57*B57</f>
-        <v>4518.2</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <f aca="false">B48</f>
-        <v>4</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <f aca="false">C58*B58</f>
-        <v>9036.4</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <f aca="false">B49</f>
-        <v>6</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D59" s="0" t="n">
-        <f aca="false">C59*B59</f>
-        <v>13554.6</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <f aca="false">B50</f>
-        <v>6</v>
-      </c>
-      <c r="C60" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D60" s="0" t="n">
-        <f aca="false">C60*B60</f>
-        <v>13554.6</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <f aca="false">B51</f>
-        <v>4</v>
-      </c>
-      <c r="C61" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D61" s="0" t="n">
-        <f aca="false">C61*B61</f>
-        <v>9036.4</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <f aca="false">B52</f>
-        <v>7</v>
-      </c>
-      <c r="C62" s="0" t="n">
-        <f aca="false">$B$42</f>
-        <v>2259.1</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <f aca="false">C62*B62</f>
+      <c r="D113" s="0" t="n">
+        <f aca="false">C113*B113</f>
         <v>15813.7</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B67:D67"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>